<commit_message>
Add c_family entry with an external reference link on C# compiling
</commit_message>
<xml_diff>
--- a/c_family_lib.xlsx
+++ b/c_family_lib.xlsx
@@ -125,18 +125,6 @@
   System.out.println(t.getVersion());
     }
 }</t>
-  </si>
-  <si>
-    <t>## Compiles to executables
-1. Build *.cs file
-1. run cmd: `csc /out:pgm.exe csdemo.cs`
-1. run executable: `./pgm`
-## Compiles to DLL library
-1. Build *.cs file
-1. run cmd: `csc /target:library csdemo.cs`
-## External Dependency Injection
-- Dependency in *using xxx*: `csc /out:pgm.exe pingLM.cs /r:FreeImageNET.dll`
-- Dependency in [DllImport...], because it is a runtime dll binding, so only need to ensure that dll is available in the same directory that pgm.exe is invoked.</t>
   </si>
   <si>
     <t>How to compile (exe, dll)</t>
@@ -225,6 +213,19 @@
        public IntPtr praw_data;
     }
 }</t>
+  </si>
+  <si>
+    <t>ref: https://www.codetuts.tech/compile-c-sharp-command-line/
+## Compiles to executables
+1. Build *.cs file
+1. run cmd: `csc /out:pgm.exe csdemo.cs`
+1. run executable: `./pgm`
+## Compiles to DLL library
+1. Build *.cs file
+1. run cmd: `csc /target:library csdemo.cs`
+## External Dependency Injection
+- Dependency in *using xxx*: `csc /out:pgm.exe pingLM.cs /r:FreeImageNET.dll`
+- Dependency in [DllImport...], because it is a runtime dll binding, so only need to ensure that dll is available in the same directory that pgm.exe is invoked.</t>
   </si>
 </sst>
 </file>
@@ -589,7 +590,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -659,10 +660,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57" customHeight="1">
@@ -670,10 +671,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add c entry basics
</commit_message>
<xml_diff>
--- a/c_family_lib.xlsx
+++ b/c_family_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Language</t>
   </si>
@@ -227,6 +227,129 @@
 - Dependency in *using xxx*: `csc /out:pgm.exe pingLM.cs /r:FreeImageNET.dll`
 - Dependency in [DllImport...], because it is a runtime dll binding, so only need to ensure that dll is available in the same directory that pgm.exe is invoked.</t>
   </si>
+  <si>
+    <t># C</t>
+  </si>
+  <si>
+    <t>## Hello world</t>
+  </si>
+  <si>
+    <t>### Hello code
+```c
+#include &lt;stdio.h&gt;
+int main() {
+   printf("Hello, World! \n");
+   return 0;
+}
+```
+### Compile
+1. Compile to exe: `cc demo.c`
+1. Compile to exe: `gcc demo.c`</t>
+  </si>
+  <si>
+    <t>## Pointer basic</t>
+  </si>
+  <si>
+    <t>#include &lt;stdio.h&gt;
+int main() {
+    int var = 20;
+    int *ip;
+    ip = &amp;var;
+    printf("Adress of var: %x\n", &amp;var );
+    printf("Adress stored in pointer ip: %x\n", ip );
+    printf("Value of *ip: %d\n", *ip );
+    return 0;
+}</t>
+  </si>
+  <si>
+    <t>#include &lt;stdio.h&gt;
+#include &lt;string.h&gt;
+struct Books {
+   char  title[50];
+   char  author[50];
+   char  subject[100];
+   int   book_id;
+};
+int main( ) {
+   struct Books Book1;        /* Declare Book1 of type Book */
+   struct Books Book2;        /* Declare Book2 of type Book */
+   /* book 1 specification */
+   strcpy( Book1.title, "C Programming");
+   strcpy( Book1.author, "Nuha Ali"); 
+   strcpy( Book1.subject, "C Programming Tutorial");
+   Book1.book_id = 6495407;</t>
+  </si>
+  <si>
+    <t>## Struct</t>
+  </si>
+  <si>
+    <t>#include &lt;stdio.h&gt;
+#include &lt;string.h&gt;
+int main () {
+   char str1[12] = "Hello";
+   char str2[12] = "World";
+   char str3[12];
+   int  len ;
+   /* copy str1 into str3 */
+   strcpy(str3, str1);
+   printf("strcpy( str3, str1) :  %s\n", str3 );
+   /* concatenates str1 and str2 */
+   strcat( str1, str2);
+   printf("strcat( str1, str2):   %s\n", str1 );
+   /* total lenghth of str1 after concatenation */
+   len = strlen(str1);
+   printf("strlen(str1) :  %d\n", len );
+   return 0;
+}</t>
+  </si>
+  <si>
+    <t>## String == char[]</t>
+  </si>
+  <si>
+    <t>## Pass pointer (int)</t>
+  </si>
+  <si>
+    <t>## Pass pointer (array)</t>
+  </si>
+  <si>
+    <t>#include &lt;stdio.h&gt;
+/* function declaration */
+double getAverage(int *arr, int size);
+int main () {
+   /* an int array with 5 elements */
+   int balance[5] = {1000, 2, 3, 17, 50};
+   double avg;
+   /* pass pointer to the array as an argument */
+   avg = getAverage( balance, 5 ) ;
+   /* output the returned value  */
+   printf("Average value is: %f\n", avg );
+   return 0;
+}
+double getAverage(int *arr, int size) {
+   int  i, sum = 0;       
+   double avg;          
+   for (i = 0; i &lt; size; ++i) {
+      sum += arr[i];
+   }
+   avg = (double)sum / size;
+   return avg;
+}</t>
+  </si>
+  <si>
+    <t>#include &lt;stdio.h&gt;
+#include &lt;time.h&gt;
+void getSeconds(unsigned long *par);
+int main () {
+   unsigned long sec;
+   getSeconds( &amp;sec );
+   printf("Number of seconds: %ld\n", sec );
+   return 0;
+}
+void getSeconds(unsigned long *par) {
+   *par = time( NULL );
+   return;
+}</t>
+  </si>
 </sst>
 </file>
 
@@ -281,11 +404,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -587,94 +707,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="47.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="72.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="72.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57" customHeight="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="63.75" customHeight="1">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57" customHeight="1">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="57" customHeight="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57" customHeight="1">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="158.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add c entry on c header file usage
</commit_message>
<xml_diff>
--- a/c_family_lib.xlsx
+++ b/c_family_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Language</t>
   </si>
@@ -349,6 +349,102 @@
    *par = time( NULL );
    return;
 }</t>
+  </si>
+  <si>
+    <t>## Create my header (BEGINER)</t>
+  </si>
+  <si>
+    <t>## Create my header (ADVANCED)</t>
+  </si>
+  <si>
+    <t>## Header</t>
+  </si>
+  <si>
+    <t>* #include &lt;file&gt; //compile look for header in __SYSTEM__ DIRECTORY
+* #include "file"  //coompiler look for header in __CURRENT__ DIRECOTRY
+* It is ok to compile without header impl, as long as the impl of header is present when program is called
+* The compilation is __stupid__, merely just copy the headers into the target program...</t>
+  </si>
+  <si>
+    <t>### Prepare myheader.h and its content is:
+```c
+int add(int a,int b)
+{
+return(a+b);
+}
+```
+### Prepare the main program main.c:
+```c
+#include&lt;stdio.h&gt;
+#include"myhead.h"
+void main() {
+   int num1 = 10, num2 = 10, num3;
+   num3 = add(num1, num2);
+   printf("Addition of Two numbers : %d", num3);
+}
+```
+### Compile 
+`cc main.c`  (must ensure myheader.h at the current folder)
+### Run
+`./a.exe`</t>
+  </si>
+  <si>
+    <t>### Prepare header file "insertion_sort.h"
+```c
+//insertion_sort.h file
+#ifndef _insertion_sort_h
+#define _insertion_sort_h
+/*Sorts an integer array. Takes a pointer to the first element and the length of the array as input. 
+Returns 0 on successful sort.*/
+int insertion_sort(int*, int); 
+#endif
+```
+### Prepare header impl "insertion_sort.c"
+```c
+//insertion_sort.c file
+#include "insertion_sort.h"
+int insertion_sort(int *a, int n){
+ int i=1;
+ int j=i;
+ int t;
+ for(i=1; i&lt;n; ++i){
+  for(j=0; j&lt;i; ++j){
+   if(a[i]&lt;a[j]){
+    t = a[i];
+    a[i] = a[j];
+    a[j] = t;
+   }
+  }
+ }
+ return 0;
+}
+```
+### Prepare the main "insertion_main.c"
+```c
+//insertion_main.c file
+#include &lt;stdio.h&gt;
+#include "insertion_sort.h"
+void print_array(int*, int);
+int main(){
+ int a[] = {10, 9, 8, 7, 6, 5, 4, 3, 2, 1};
+ insertion_sort(a, 10);
+ print_array(a, 10);
+}
+void print_array(int *arr, int n){
+ int i;
+ for(i=0; i&lt;n; ++i){
+  printf("%d ", arr[i]);
+ }
+}
+```
+### Compile 
+```bash
+cc -c insertion_sort.c #this will give you insertion_sort.o
+cc -c insertion_main.c #this will give you insertion_main.o
+cc -o insertion_main insertion_main.o insertion_sort.o #this will create the insertion_main executable
+```
+### Run
+`./insertion_main`</t>
   </si>
 </sst>
 </file>
@@ -707,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="47.25" customHeight="1"/>
@@ -861,6 +957,39 @@
       </c>
       <c r="C13" s="3" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="47.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>